<commit_message>
Mise en forme (à finir)
</commit_message>
<xml_diff>
--- a/Documents/RéponsePétut.xlsx
+++ b/Documents/RéponsePétut.xlsx
@@ -199,8 +199,3618 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="378">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF00FFFF"/>
+      <color rgb="FFFF99CC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -479,12 +4089,14 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M14" sqref="M14"/>
+      <selection pane="bottomLeft" activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="11" width="21.5703125" customWidth="1"/>
+    <col min="1" max="9" width="21.5703125" customWidth="1"/>
+    <col min="10" max="10" width="23" customWidth="1"/>
+    <col min="11" max="11" width="30" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5385,6 +8997,104 @@
   <sortState ref="A1:K214">
     <sortCondition ref="D1"/>
   </sortState>
+  <conditionalFormatting sqref="F2:F96">
+    <cfRule type="containsText" dxfId="52" priority="27" operator="containsText" text="Oui">
+      <formula>NOT(ISERROR(SEARCH("Oui",F2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="51" priority="26" operator="containsText" text="peu">
+      <formula>NOT(ISERROR(SEARCH("peu",F2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="50" priority="25" operator="containsText" text="Non">
+      <formula>NOT(ISERROR(SEARCH("Non",F2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="containsText" dxfId="49" priority="24" operator="containsText" text="base">
+      <formula>NOT(ISERROR(SEARCH("base",G1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="48" priority="23" operator="containsText" text="aucun">
+      <formula>NOT(ISERROR(SEARCH("aucun",G1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="47" priority="22" operator="containsText" text="avancé">
+      <formula>NOT(ISERROR(SEARCH("avancé",G1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="46" priority="21" operator="containsText" text="expert">
+      <formula>NOT(ISERROR(SEARCH("expert",G1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="45" priority="20" operator="containsText" text="base">
+      <formula>NOT(ISERROR(SEARCH("base",G1)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="19" operator="equal">
+      <formula>"avancé"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="43" priority="18" operator="equal">
+      <formula>"expert"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="42" priority="7" operator="containsText" text="base">
+      <formula>NOT(ISERROR(SEARCH("base",G1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="41" priority="6" operator="containsText" text="base">
+      <formula>NOT(ISERROR(SEARCH("base",G1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H1048576">
+    <cfRule type="containsText" dxfId="40" priority="17" operator="containsText" text="base">
+      <formula>NOT(ISERROR(SEARCH("base",H1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="39" priority="16" operator="containsText" text="avancé">
+      <formula>NOT(ISERROR(SEARCH("avancé",H1)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="15" operator="equal">
+      <formula>"expert"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I1:I1048576">
+    <cfRule type="containsText" dxfId="37" priority="14" operator="containsText" text="Oui">
+      <formula>NOT(ISERROR(SEARCH("Oui",I1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="36" priority="13" operator="containsText" text="Non,">
+      <formula>NOT(ISERROR(SEARCH("Non,",I1)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="35" priority="12" operator="equal">
+      <formula>"Non"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J1:J1048576">
+    <cfRule type="cellIs" dxfId="34" priority="11" operator="equal">
+      <formula>"Oui"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="33" priority="10" operator="containsText" text="Non,">
+      <formula>NOT(ISERROR(SEARCH("Non,",J1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="32" priority="9" operator="containsText" text="Non">
+      <formula>NOT(ISERROR(SEARCH("Non",J1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="31" priority="8" operator="containsText" text="Non,">
+      <formula>NOT(ISERROR(SEARCH("Non,",J1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K1:K1048576">
+    <cfRule type="containsText" dxfId="30" priority="5" operator="containsText" text="Non">
+      <formula>NOT(ISERROR(SEARCH("Non",K1)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="4" operator="equal">
+      <formula>"Oui"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="containsText" dxfId="28" priority="3" operator="containsText" text="F">
+      <formula>NOT(ISERROR(SEARCH("F",C1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="27" priority="2" operator="containsText" text="M">
+      <formula>NOT(ISERROR(SEARCH("M",C1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Aucun">
+      <formula>NOT(ISERROR(SEARCH("Aucun",E1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fin tri par couleur
</commit_message>
<xml_diff>
--- a/Documents/RéponsePétut.xlsx
+++ b/Documents/RéponsePétut.xlsx
@@ -166,7 +166,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -175,6 +175,11 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -197,16 +202,4111 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="435">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF33CCFF"/>
+      <color rgb="FFFF99CC"/>
+      <color rgb="FFFFFF99"/>
+      <color rgb="FFFF99FF"/>
+      <color rgb="FFFF6699"/>
+      <color rgb="FF00FFFF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -485,12 +4585,21 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomLeft" activeCell="E121" sqref="E121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="11" width="21.5703125" customWidth="1"/>
+    <col min="1" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="65.5703125" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" customWidth="1"/>
+    <col min="11" max="11" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -532,7 +4641,7 @@
       <c r="A2" s="1">
         <v>42493.581549456023</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -4662,6 +8771,112 @@
   <sortState ref="A2:K214">
     <sortCondition ref="E1"/>
   </sortState>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="containsText" dxfId="56" priority="29" operator="containsText" text="Non">
+      <formula>NOT(ISERROR(SEARCH("Non",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="55" priority="28" operator="containsText" text="OUI">
+      <formula>NOT(ISERROR(SEARCH("OUI",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="containsText" dxfId="54" priority="27" operator="containsText" text="M">
+      <formula>NOT(ISERROR(SEARCH("M",C1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="53" priority="26" operator="containsText" text="F">
+      <formula>NOT(ISERROR(SEARCH("F",C1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="containsText" dxfId="52" priority="25" operator="containsText" text="Non">
+      <formula>NOT(ISERROR(SEARCH("Non",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="51" priority="24" operator="containsText" text="Un">
+      <formula>NOT(ISERROR(SEARCH("Un",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="50" priority="23" operator="containsText" text="Oui">
+      <formula>NOT(ISERROR(SEARCH("Oui",F1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="containsText" dxfId="49" priority="22" operator="containsText" text="aucun">
+      <formula>NOT(ISERROR(SEARCH("aucun",G1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="48" priority="21" operator="containsText" text="base">
+      <formula>NOT(ISERROR(SEARCH("base",G1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="47" priority="20" operator="containsText" text="ava">
+      <formula>NOT(ISERROR(SEARCH("ava",G1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="46" priority="19" operator="containsText" text="exp">
+      <formula>NOT(ISERROR(SEARCH("exp",G1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H1048576">
+    <cfRule type="containsText" dxfId="45" priority="18" operator="containsText" text="base">
+      <formula>NOT(ISERROR(SEARCH("base",H1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="44" priority="17" operator="containsText" text="ava">
+      <formula>NOT(ISERROR(SEARCH("ava",H1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="43" priority="16" operator="containsText" text="ex">
+      <formula>NOT(ISERROR(SEARCH("ex",H1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I1:I1048576">
+    <cfRule type="containsText" dxfId="42" priority="15" operator="containsText" text="Oui">
+      <formula>NOT(ISERROR(SEARCH("Oui",I1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="41" priority="14" operator="containsText" text="Non">
+      <formula>NOT(ISERROR(SEARCH("Non",I1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="40" priority="13" operator="containsText" text="Non,">
+      <formula>NOT(ISERROR(SEARCH("Non,",I1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J1:J1048576">
+    <cfRule type="containsText" dxfId="39" priority="12" operator="containsText" text="Oui">
+      <formula>NOT(ISERROR(SEARCH("Oui",J1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="38" priority="11" operator="containsText" text="Non">
+      <formula>NOT(ISERROR(SEARCH("Non",J1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="37" priority="10" operator="containsText" text="Non,">
+      <formula>NOT(ISERROR(SEARCH("Non,",J1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K1:K1048576">
+    <cfRule type="containsText" dxfId="36" priority="9" operator="containsText" text="Oui">
+      <formula>NOT(ISERROR(SEARCH("Oui",K1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="35" priority="8" operator="containsText" text="Non">
+      <formula>NOT(ISERROR(SEARCH("Non",K1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="containsText" dxfId="0" priority="7" operator="containsText" text="moins">
+      <formula>NOT(ISERROR(SEARCH("moins",B1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="6" operator="containsText" text="15 à 18">
+      <formula>NOT(ISERROR(SEARCH("15 à 18",B1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text=" 18 à 25 ">
+      <formula>NOT(ISERROR(SEARCH(" 18 à 25 ",B1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="30 à 40">
+      <formula>NOT(ISERROR(SEARCH("30 à 40",B1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="30 à 40">
+      <formula>NOT(ISERROR(SEARCH("30 à 40",B1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="40 à 60">
+      <formula>NOT(ISERROR(SEARCH("40 à 60",B1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="plus">
+      <formula>NOT(ISERROR(SEARCH("plus",B1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>